<commit_message>
adding more and more
</commit_message>
<xml_diff>
--- a/target/test-classes/data/userData.xlsx
+++ b/target/test-classes/data/userData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13065" windowHeight="4155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="2670"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,10 @@
     <t>test1</t>
   </si>
   <si>
-    <t>es234@yahoo.com</t>
-  </si>
-  <si>
-    <t>us1234@test.com</t>
+    <t>es2345@yahoo.com</t>
+  </si>
+  <si>
+    <t>us12345@test.com</t>
   </si>
 </sst>
 </file>

</xml_diff>